<commit_message>
[ENF] Add Report and reformat
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_monthly_work_acceptance.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_monthly_work_acceptance.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -41,9 +41,6 @@
     <t>วันที่ PO</t>
   </si>
   <si>
-    <t>Header Text ที่โยนมาจาก PR</t>
-  </si>
-  <si>
     <t>รหัสแหล่งงบประมาณ</t>
   </si>
   <si>
@@ -84,13 +81,23 @@
   </si>
   <si>
     <t>ถึงวันที่</t>
+  </si>
+  <si>
+    <t>ศูนย์</t>
+  </si>
+  <si>
+    <t>รายละเอียดการซื้อจ้าง</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,23 +105,32 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,21 +189,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -195,6 +272,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -463,164 +543,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="25" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" style="23" customWidth="1"/>
+    <col min="5" max="8" width="25.54296875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" style="10" customWidth="1"/>
+    <col min="10" max="12" width="25.54296875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="25.54296875" style="23" customWidth="1"/>
+    <col min="14" max="14" width="25.54296875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="25.54296875" style="23" customWidth="1"/>
+    <col min="16" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="20"/>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="20"/>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" s="16" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="B5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
-    <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.60972222222222205" bottom="0.37013888888888902" header="0.51180555555555496" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;8 2018-02-20 09:37:39&amp;R&amp;8&amp;P / &amp;N</oddFooter>
   </headerFooter>

</xml_diff>